<commit_message>
2018.09.15 - Level tweaks & Debug Mode (Key:Z)
</commit_message>
<xml_diff>
--- a/res/levels/Level_1-1.xlsx
+++ b/res/levels/Level_1-1.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\luigi-game\luigi-game\res\levels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{60E58D0B-5D50-43B3-8EC2-14A52A4A8BB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{90D58B6D-124E-45C1-8813-4ECAD9BB8A8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3E10F1A8-61DE-4F73-969A-005C05217034}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11210" windowHeight="1130" xr2:uid="{3E10F1A8-61DE-4F73-969A-005C05217034}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -668,17 +664,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B0B742-47D3-459D-A686-B8228BA77617}">
   <dimension ref="A1:HD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FD1" workbookViewId="0">
-      <selection activeCell="GV11" sqref="GV11"/>
+    <sheetView tabSelected="1" topLeftCell="GL5" workbookViewId="0">
+      <selection activeCell="GR5" sqref="GR5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="212" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:212" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:212" x14ac:dyDescent="0.35">
       <c r="B1" s="16">
         <v>1</v>
       </c>
@@ -1313,7 +1309,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>22</v>
       </c>
@@ -1951,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>23</v>
       </c>
@@ -2589,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
@@ -3227,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>25</v>
       </c>
@@ -3819,11 +3815,11 @@
       <c r="GO5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="GP5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="GQ5" s="14" t="s">
+      <c r="GP5" s="14" t="s">
         <v>40</v>
+      </c>
+      <c r="GQ5" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="GR5" s="2" t="s">
         <v>0</v>
@@ -3865,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>27</v>
       </c>
@@ -5141,7 +5137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
@@ -5779,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>29</v>
       </c>
@@ -6417,7 +6413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
@@ -7055,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>31</v>
       </c>
@@ -7693,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -8331,7 +8327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>33</v>
       </c>
@@ -8969,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>34</v>
       </c>
@@ -9607,7 +9603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
@@ -10245,7 +10241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:212" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
@@ -10895,7 +10891,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10907,7 +10903,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10919,7 +10915,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2018.09.24 - Added Pipe Level to Level 1-1 (and imported all tiles)
</commit_message>
<xml_diff>
--- a/res/levels/Level_1-1.xlsx
+++ b/res/levels/Level_1-1.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{720EFC51-1B73-40DE-BAEE-201DFDA4FDAC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\luigi-game\luigi-game\res\levels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C5B77BEF-F0A1-4C10-B068-890282B8F0AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16020" windowHeight="3720" xr2:uid="{3E10F1A8-61DE-4F73-969A-005C05217034}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16020" windowHeight="3720" xr2:uid="{3E10F1A8-61DE-4F73-969A-005C05217034}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="World 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3180" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3675" uniqueCount="57">
   <si>
     <t>0550</t>
   </si>
@@ -169,6 +170,33 @@
   <si>
     <t>0569</t>
   </si>
+  <si>
+    <t>0570</t>
+  </si>
+  <si>
+    <t>0063</t>
+  </si>
+  <si>
+    <t>0061</t>
+  </si>
+  <si>
+    <t>0246</t>
+  </si>
+  <si>
+    <t>0247</t>
+  </si>
+  <si>
+    <t>0248</t>
+  </si>
+  <si>
+    <t>0272</t>
+  </si>
+  <si>
+    <t>0273</t>
+  </si>
+  <si>
+    <t>0274</t>
+  </si>
 </sst>
 </file>
 
@@ -198,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +318,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2894AE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3AB5D2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -318,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -341,6 +381,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,8 +394,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF6AB212"/>
       <color rgb="FF99EB35"/>
-      <color rgb="FF6AB212"/>
+      <color rgb="FF3AB5D2"/>
+      <color rgb="FF2894AE"/>
       <color rgb="FFC1DA46"/>
     </mruColors>
   </colors>
@@ -662,19 +709,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B0B742-47D3-459D-A686-B8228BA77617}">
-  <dimension ref="A1:HD16"/>
+  <dimension ref="A1:HT33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="212" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="228" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:212" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:228" x14ac:dyDescent="0.25">
       <c r="B1" s="15">
         <v>1</v>
       </c>
@@ -1308,8 +1355,56 @@
       <c r="HD1" s="15">
         <v>211</v>
       </c>
+      <c r="HE1" s="15">
+        <v>212</v>
+      </c>
+      <c r="HF1" s="15">
+        <v>213</v>
+      </c>
+      <c r="HG1" s="15">
+        <v>214</v>
+      </c>
+      <c r="HH1" s="15">
+        <v>215</v>
+      </c>
+      <c r="HI1" s="15">
+        <v>216</v>
+      </c>
+      <c r="HJ1" s="15">
+        <v>217</v>
+      </c>
+      <c r="HK1" s="15">
+        <v>218</v>
+      </c>
+      <c r="HL1" s="15">
+        <v>219</v>
+      </c>
+      <c r="HM1" s="15">
+        <v>220</v>
+      </c>
+      <c r="HN1" s="15">
+        <v>221</v>
+      </c>
+      <c r="HO1" s="15">
+        <v>222</v>
+      </c>
+      <c r="HP1" s="15">
+        <v>223</v>
+      </c>
+      <c r="HQ1" s="15">
+        <v>224</v>
+      </c>
+      <c r="HR1" s="15">
+        <v>225</v>
+      </c>
+      <c r="HS1" s="15">
+        <v>226</v>
+      </c>
+      <c r="HT1" s="15">
+        <v>227</v>
+      </c>
     </row>
-    <row r="2" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -1946,8 +2041,56 @@
       <c r="HD2" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT2" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
@@ -2584,8 +2727,56 @@
       <c r="HD3" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT3" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -3222,8 +3413,56 @@
       <c r="HD4" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HJ4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HK4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HL4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HM4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HN4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HO4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HP4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT4" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
@@ -3860,8 +4099,56 @@
       <c r="HD5" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT5" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>25</v>
       </c>
@@ -4498,8 +4785,56 @@
       <c r="HD6" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT6" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -5136,8 +5471,56 @@
       <c r="HD7" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT7" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>27</v>
       </c>
@@ -5774,8 +6157,56 @@
       <c r="HD8" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT8" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="9" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -6412,8 +6843,56 @@
       <c r="HD9" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT9" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
@@ -7050,8 +7529,56 @@
       <c r="HD10" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT10" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>30</v>
       </c>
@@ -7688,8 +8215,56 @@
       <c r="HD11" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE11" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HJ11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HK11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HL11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HM11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HN11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HO11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HP11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT11" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
@@ -8326,8 +8901,56 @@
       <c r="HD12" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HJ12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HK12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HL12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HM12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HN12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HO12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HP12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HS12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HT12" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="13" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>32</v>
       </c>
@@ -8964,8 +9587,56 @@
       <c r="HD13" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HJ13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HK13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HL13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HM13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HN13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HO13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HP13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="HS13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="HT13" s="22" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="14" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>33</v>
       </c>
@@ -9602,8 +10273,56 @@
       <c r="HD14" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="HE14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HF14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HG14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HH14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HI14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HJ14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HK14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HL14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HM14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HN14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HO14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="HP14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HQ14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="HR14" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="HS14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="HT14" s="21" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="15" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>34</v>
       </c>
@@ -10240,8 +10959,56 @@
       <c r="HD15" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="HE15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HF15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HG15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HH15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HI15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HJ15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HK15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HL15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HM15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HN15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HO15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HP15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HQ15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HR15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HS15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HT15" s="20" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="16" spans="1:212" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
@@ -10877,46 +11644,1536 @@
       </c>
       <c r="HD16" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="HE16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HF16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HG16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HH16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HI16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HJ16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HK16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HL16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HM16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HN16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HO16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HP16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HQ16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HR16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HS16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="HT16" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:228" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>1</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3</v>
+      </c>
+      <c r="E18" s="15">
+        <v>4</v>
+      </c>
+      <c r="F18" s="15">
+        <v>5</v>
+      </c>
+      <c r="G18" s="15">
+        <v>6</v>
+      </c>
+      <c r="H18" s="15">
+        <v>7</v>
+      </c>
+      <c r="I18" s="15">
+        <v>8</v>
+      </c>
+      <c r="J18" s="15">
+        <v>9</v>
+      </c>
+      <c r="K18" s="15">
+        <v>10</v>
+      </c>
+      <c r="L18" s="15">
+        <v>11</v>
+      </c>
+      <c r="M18" s="15">
+        <v>12</v>
+      </c>
+      <c r="N18" s="15">
+        <v>13</v>
+      </c>
+      <c r="O18" s="15">
+        <v>14</v>
+      </c>
+      <c r="P18" s="15">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="15">
+        <v>16</v>
+      </c>
+      <c r="R18" s="15">
+        <v>17</v>
+      </c>
+      <c r="S18" s="15">
+        <v>18</v>
+      </c>
+      <c r="T18" s="15">
+        <v>19</v>
+      </c>
+      <c r="U18" s="15">
+        <v>20</v>
+      </c>
+      <c r="V18" s="15">
+        <v>21</v>
+      </c>
+      <c r="W18" s="15">
+        <v>22</v>
+      </c>
+      <c r="X18" s="15">
+        <v>23</v>
+      </c>
+      <c r="Y18" s="15">
+        <v>24</v>
+      </c>
+      <c r="Z18" s="15">
+        <v>25</v>
+      </c>
+      <c r="AA18" s="15">
+        <v>26</v>
+      </c>
+      <c r="AB18" s="15">
+        <v>27</v>
+      </c>
+      <c r="AC18" s="15">
+        <v>28</v>
+      </c>
+      <c r="AD18" s="15">
+        <v>29</v>
+      </c>
+      <c r="AE18" s="15">
+        <v>30</v>
+      </c>
+      <c r="AF18" s="15">
+        <v>31</v>
+      </c>
+      <c r="AG18" s="15">
+        <v>32</v>
+      </c>
+      <c r="AH18" s="15">
+        <v>33</v>
+      </c>
+      <c r="AI18" s="15">
+        <v>34</v>
+      </c>
+      <c r="AJ18" s="15">
+        <v>35</v>
+      </c>
+      <c r="AK18" s="15">
+        <v>36</v>
+      </c>
+      <c r="AL18" s="15">
+        <v>37</v>
+      </c>
+      <c r="AM18" s="15">
+        <v>38</v>
+      </c>
+      <c r="AN18" s="15">
+        <v>39</v>
+      </c>
+      <c r="AO18" s="15">
+        <v>40</v>
+      </c>
+      <c r="AP18" s="15">
+        <v>41</v>
+      </c>
+      <c r="AQ18" s="15">
+        <v>42</v>
+      </c>
+      <c r="AR18" s="15">
+        <v>43</v>
+      </c>
+      <c r="AS18" s="15">
+        <v>44</v>
+      </c>
+      <c r="AT18" s="15">
+        <v>45</v>
+      </c>
+      <c r="AU18" s="15">
+        <v>46</v>
+      </c>
+      <c r="AV18" s="15">
+        <v>47</v>
+      </c>
+      <c r="AW18" s="15">
+        <v>48</v>
+      </c>
+      <c r="AX18" s="15">
+        <v>49</v>
+      </c>
+      <c r="AY18" s="15">
+        <v>50</v>
+      </c>
+      <c r="AZ18" s="15">
+        <v>51</v>
+      </c>
+      <c r="BA18" s="15">
+        <v>52</v>
+      </c>
+      <c r="BB18" s="15">
+        <v>53</v>
+      </c>
+      <c r="BC18" s="15">
+        <v>54</v>
+      </c>
+      <c r="BD18" s="15">
+        <v>55</v>
+      </c>
+      <c r="BE18" s="15">
+        <v>56</v>
+      </c>
+      <c r="BF18" s="15">
+        <v>57</v>
+      </c>
+      <c r="BG18" s="15">
+        <v>58</v>
+      </c>
+      <c r="BH18" s="15">
+        <v>59</v>
+      </c>
+      <c r="BI18" s="15">
+        <v>60</v>
+      </c>
+      <c r="BJ18" s="15">
+        <v>61</v>
+      </c>
+      <c r="BK18" s="15">
+        <v>62</v>
+      </c>
+      <c r="BL18" s="15">
+        <v>63</v>
+      </c>
+      <c r="BM18" s="15">
+        <v>64</v>
+      </c>
+      <c r="BN18" s="15">
+        <v>65</v>
+      </c>
+      <c r="BO18" s="15">
+        <v>66</v>
+      </c>
+      <c r="BP18" s="15">
+        <v>67</v>
+      </c>
+      <c r="BQ18" s="15">
+        <v>68</v>
+      </c>
+      <c r="BR18" s="15">
+        <v>69</v>
+      </c>
+      <c r="BS18" s="15">
+        <v>70</v>
+      </c>
+      <c r="BT18" s="15">
+        <v>71</v>
+      </c>
+      <c r="BU18" s="15">
+        <v>72</v>
+      </c>
+      <c r="BV18" s="15">
+        <v>73</v>
+      </c>
+      <c r="BW18" s="15">
+        <v>74</v>
+      </c>
+      <c r="BX18" s="15">
+        <v>75</v>
+      </c>
+      <c r="BY18" s="15">
+        <v>76</v>
+      </c>
+      <c r="BZ18" s="15">
+        <v>77</v>
+      </c>
+      <c r="CA18" s="15">
+        <v>78</v>
+      </c>
+      <c r="CB18" s="15">
+        <v>79</v>
+      </c>
+      <c r="CC18" s="15">
+        <v>80</v>
+      </c>
+      <c r="CD18" s="15">
+        <v>81</v>
+      </c>
+      <c r="CE18" s="15">
+        <v>82</v>
+      </c>
+      <c r="CF18" s="15">
+        <v>83</v>
+      </c>
+      <c r="CG18" s="15">
+        <v>84</v>
+      </c>
+      <c r="CH18" s="15">
+        <v>85</v>
+      </c>
+      <c r="CI18" s="15">
+        <v>86</v>
+      </c>
+      <c r="CJ18" s="15">
+        <v>87</v>
+      </c>
+      <c r="CK18" s="15">
+        <v>88</v>
+      </c>
+      <c r="CL18" s="15">
+        <v>89</v>
+      </c>
+      <c r="CM18" s="15">
+        <v>90</v>
+      </c>
+      <c r="CN18" s="15">
+        <v>91</v>
+      </c>
+      <c r="CO18" s="15">
+        <v>92</v>
+      </c>
+      <c r="CP18" s="15">
+        <v>93</v>
+      </c>
+      <c r="CQ18" s="15">
+        <v>94</v>
+      </c>
+      <c r="CR18" s="15">
+        <v>95</v>
+      </c>
+      <c r="CS18" s="15">
+        <v>96</v>
+      </c>
+      <c r="CT18" s="15">
+        <v>97</v>
+      </c>
+      <c r="CU18" s="15">
+        <v>98</v>
+      </c>
+      <c r="CV18" s="15">
+        <v>99</v>
+      </c>
+      <c r="CW18" s="15">
+        <v>100</v>
+      </c>
+      <c r="CX18" s="15">
+        <v>101</v>
+      </c>
+      <c r="CY18" s="15">
+        <v>102</v>
+      </c>
+      <c r="CZ18" s="15">
+        <v>103</v>
+      </c>
+      <c r="DA18" s="15">
+        <v>104</v>
+      </c>
+      <c r="DB18" s="15">
+        <v>105</v>
+      </c>
+      <c r="DC18" s="15">
+        <v>106</v>
+      </c>
+      <c r="DD18" s="15">
+        <v>107</v>
+      </c>
+      <c r="DE18" s="15">
+        <v>108</v>
+      </c>
+      <c r="DF18" s="15">
+        <v>109</v>
+      </c>
+      <c r="DG18" s="15">
+        <v>110</v>
+      </c>
+      <c r="DH18" s="15">
+        <v>111</v>
+      </c>
+      <c r="DI18" s="15">
+        <v>112</v>
+      </c>
+      <c r="DJ18" s="15">
+        <v>113</v>
+      </c>
+      <c r="DK18" s="15">
+        <v>114</v>
+      </c>
+      <c r="DL18" s="15">
+        <v>115</v>
+      </c>
+      <c r="DM18" s="15">
+        <v>116</v>
+      </c>
+      <c r="DN18" s="15">
+        <v>117</v>
+      </c>
+      <c r="DO18" s="15">
+        <v>118</v>
+      </c>
+      <c r="DP18" s="15">
+        <v>119</v>
+      </c>
+      <c r="DQ18" s="15">
+        <v>120</v>
+      </c>
+      <c r="DR18" s="15">
+        <v>121</v>
+      </c>
+      <c r="DS18" s="15">
+        <v>122</v>
+      </c>
+      <c r="DT18" s="15">
+        <v>123</v>
+      </c>
+      <c r="DU18" s="15">
+        <v>124</v>
+      </c>
+      <c r="DV18" s="15">
+        <v>125</v>
+      </c>
+      <c r="DW18" s="15">
+        <v>126</v>
+      </c>
+      <c r="DX18" s="15">
+        <v>127</v>
+      </c>
+      <c r="DY18" s="15">
+        <v>128</v>
+      </c>
+      <c r="DZ18" s="15">
+        <v>129</v>
+      </c>
+      <c r="EA18" s="15">
+        <v>130</v>
+      </c>
+      <c r="EB18" s="15">
+        <v>131</v>
+      </c>
+      <c r="EC18" s="15">
+        <v>132</v>
+      </c>
+      <c r="ED18" s="15">
+        <v>133</v>
+      </c>
+      <c r="EE18" s="15">
+        <v>134</v>
+      </c>
+      <c r="EF18" s="15">
+        <v>135</v>
+      </c>
+      <c r="EG18" s="15">
+        <v>136</v>
+      </c>
+      <c r="EH18" s="15">
+        <v>137</v>
+      </c>
+      <c r="EI18" s="15">
+        <v>138</v>
+      </c>
+      <c r="EJ18" s="15">
+        <v>139</v>
+      </c>
+      <c r="EK18" s="15">
+        <v>140</v>
+      </c>
+      <c r="EL18" s="15">
+        <v>141</v>
+      </c>
+      <c r="EM18" s="15">
+        <v>142</v>
+      </c>
+      <c r="EN18" s="15">
+        <v>143</v>
+      </c>
+      <c r="EO18" s="15">
+        <v>144</v>
+      </c>
+      <c r="EP18" s="15">
+        <v>145</v>
+      </c>
+      <c r="EQ18" s="15">
+        <v>146</v>
+      </c>
+      <c r="ER18" s="15">
+        <v>147</v>
+      </c>
+      <c r="ES18" s="15">
+        <v>148</v>
+      </c>
+      <c r="ET18" s="15">
+        <v>149</v>
+      </c>
+      <c r="EU18" s="15">
+        <v>150</v>
+      </c>
+      <c r="EV18" s="15">
+        <v>151</v>
+      </c>
+      <c r="EW18" s="15">
+        <v>152</v>
+      </c>
+      <c r="EX18" s="15">
+        <v>153</v>
+      </c>
+      <c r="EY18" s="15">
+        <v>154</v>
+      </c>
+      <c r="EZ18" s="15">
+        <v>155</v>
+      </c>
+      <c r="FA18" s="15">
+        <v>156</v>
+      </c>
+      <c r="FB18" s="15">
+        <v>157</v>
+      </c>
+      <c r="FC18" s="15">
+        <v>158</v>
+      </c>
+      <c r="FD18" s="15">
+        <v>159</v>
+      </c>
+      <c r="FE18" s="15">
+        <v>160</v>
+      </c>
+      <c r="FF18" s="15">
+        <v>161</v>
+      </c>
+      <c r="FG18" s="15">
+        <v>162</v>
+      </c>
+      <c r="FH18" s="15">
+        <v>163</v>
+      </c>
+      <c r="FI18" s="15">
+        <v>164</v>
+      </c>
+      <c r="FJ18" s="15">
+        <v>165</v>
+      </c>
+      <c r="FK18" s="15">
+        <v>166</v>
+      </c>
+      <c r="FL18" s="15">
+        <v>167</v>
+      </c>
+      <c r="FM18" s="15">
+        <v>168</v>
+      </c>
+      <c r="FN18" s="15">
+        <v>169</v>
+      </c>
+      <c r="FO18" s="15">
+        <v>170</v>
+      </c>
+      <c r="FP18" s="15">
+        <v>171</v>
+      </c>
+      <c r="FQ18" s="15">
+        <v>172</v>
+      </c>
+      <c r="FR18" s="15">
+        <v>173</v>
+      </c>
+      <c r="FS18" s="15">
+        <v>174</v>
+      </c>
+      <c r="FT18" s="15">
+        <v>175</v>
+      </c>
+      <c r="FU18" s="15">
+        <v>176</v>
+      </c>
+      <c r="FV18" s="15">
+        <v>177</v>
+      </c>
+      <c r="FW18" s="15">
+        <v>178</v>
+      </c>
+      <c r="FX18" s="15">
+        <v>179</v>
+      </c>
+      <c r="FY18" s="15">
+        <v>180</v>
+      </c>
+      <c r="FZ18" s="15">
+        <v>181</v>
+      </c>
+      <c r="GA18" s="15">
+        <v>182</v>
+      </c>
+      <c r="GB18" s="15">
+        <v>183</v>
+      </c>
+      <c r="GC18" s="15">
+        <v>184</v>
+      </c>
+      <c r="GD18" s="15">
+        <v>185</v>
+      </c>
+      <c r="GE18" s="15">
+        <v>186</v>
+      </c>
+      <c r="GF18" s="15">
+        <v>187</v>
+      </c>
+      <c r="GG18" s="15">
+        <v>188</v>
+      </c>
+      <c r="GH18" s="15">
+        <v>189</v>
+      </c>
+      <c r="GI18" s="15">
+        <v>190</v>
+      </c>
+      <c r="GJ18" s="15">
+        <v>191</v>
+      </c>
+      <c r="GK18" s="15">
+        <v>192</v>
+      </c>
+      <c r="GL18" s="15">
+        <v>193</v>
+      </c>
+      <c r="GM18" s="15">
+        <v>194</v>
+      </c>
+      <c r="GN18" s="15">
+        <v>195</v>
+      </c>
+      <c r="GO18" s="15">
+        <v>196</v>
+      </c>
+      <c r="GP18" s="15">
+        <v>197</v>
+      </c>
+      <c r="GQ18" s="15">
+        <v>198</v>
+      </c>
+      <c r="GR18" s="15">
+        <v>199</v>
+      </c>
+      <c r="GS18" s="15">
+        <v>200</v>
+      </c>
+      <c r="GT18" s="15">
+        <v>201</v>
+      </c>
+      <c r="GU18" s="15">
+        <v>202</v>
+      </c>
+      <c r="GV18" s="15">
+        <v>203</v>
+      </c>
+      <c r="GW18" s="15">
+        <v>204</v>
+      </c>
+      <c r="GX18" s="15">
+        <v>205</v>
+      </c>
+      <c r="GY18" s="15">
+        <v>206</v>
+      </c>
+      <c r="GZ18" s="15">
+        <v>207</v>
+      </c>
+      <c r="HA18" s="15">
+        <v>208</v>
+      </c>
+      <c r="HB18" s="15">
+        <v>209</v>
+      </c>
+      <c r="HC18" s="15">
+        <v>210</v>
+      </c>
+      <c r="HD18" s="15">
+        <v>211</v>
+      </c>
+      <c r="HE18" s="15">
+        <v>212</v>
+      </c>
+      <c r="HF18" s="15">
+        <v>213</v>
+      </c>
+      <c r="HG18" s="15">
+        <v>214</v>
+      </c>
+      <c r="HH18" s="15">
+        <v>215</v>
+      </c>
+      <c r="HI18" s="15">
+        <v>216</v>
+      </c>
+      <c r="HJ18" s="15">
+        <v>217</v>
+      </c>
+      <c r="HK18" s="15">
+        <v>218</v>
+      </c>
+      <c r="HL18" s="15">
+        <v>219</v>
+      </c>
+      <c r="HM18" s="15">
+        <v>220</v>
+      </c>
+      <c r="HN18" s="15">
+        <v>221</v>
+      </c>
+      <c r="HO18" s="15">
+        <v>222</v>
+      </c>
+      <c r="HP18" s="15">
+        <v>223</v>
+      </c>
+      <c r="HQ18" s="15">
+        <v>224</v>
+      </c>
+      <c r="HR18" s="15">
+        <v>225</v>
+      </c>
+      <c r="HS18" s="15">
+        <v>226</v>
+      </c>
+      <c r="HT18" s="15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q22" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q23" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q24" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P27" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q28" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O30" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="P30" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q30" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="P31" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:228" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="P32" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q32" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="N33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="P33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q33" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E4B8AA-D084-4423-8944-54D90160297C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4DA480-9DCB-4B6D-B71D-B1A3409CE7E6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1BF69D-CDBF-46DA-92B7-7B5D786B51D1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>